<commit_message>
add KIT and TUM IC Design analysis
</commit_message>
<xml_diff>
--- a/api/python/TaiGerTranscriptAnalyzerJS/database/ElectricalEngineering/EE_Programs.xlsx
+++ b/api/python/TaiGerTranscriptAnalyzerJS/database/ElectricalEngineering/EE_Programs.xlsx
@@ -8,15 +8,15 @@
   <definedNames/>
   <calcPr/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjSBblBzwlTrlfA3ayQqkVyfFq3Tw=="/>
+    <ext uri="GoogleSheetsCustomDataVersion2">
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="r5IslSnPsvXrbmeSh16L3WE84UWuRpacy2l4ZuQtbVs="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>Program</t>
   </si>
@@ -53,12 +53,18 @@
   <si>
     <t>FAU_INFO_COMM_TECH</t>
   </si>
+  <si>
+    <t>TUM_ASIA_IC_DESIGN</t>
+  </si>
+  <si>
+    <t>KIT_EI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -68,7 +74,11 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -85,13 +95,19 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -378,15 +394,29 @@
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1"/>
-    <row r="11" ht="14.25" customHeight="1"/>
+    <row r="10" ht="14.25" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" ht="14.25" customHeight="1">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="12" ht="14.25" customHeight="1"/>
     <row r="13" ht="14.25" customHeight="1"/>
     <row r="14" ht="14.25" customHeight="1"/>
@@ -1378,7 +1408,7 @@
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B1:B9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B1:B11">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>